<commit_message>
support mass unit concentrations
</commit_message>
<xml_diff>
--- a/inst/extdata/midar_metadata_templates.xlsx
+++ b/inst/extdata/midar_metadata_templates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lsibjb/Documents/Code/midar/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5098FF1-41C8-394D-9073-C5A7346A19F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1679488-CED5-304E-8E14-5C24EE10EC78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18820" yWindow="12600" windowWidth="22940" windowHeight="19140" activeTab="2" xr2:uid="{7A04E2C8-868F-5640-98CB-88D372530A12}"/>
+    <workbookView xWindow="13060" yWindow="3140" windowWidth="22940" windowHeight="19140" activeTab="2" xr2:uid="{7A04E2C8-868F-5640-98CB-88D372530A12}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="6" r:id="rId1"/>
@@ -692,7 +692,16 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional
-Used also in table QCconcentrations in which case it must match
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Used also in table QCconcentrations in which case it must match
 </t>
         </r>
       </text>
@@ -777,6 +786,34 @@
         </r>
       </text>
     </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{A41AE4CE-AE3D-0B4C-84D1-2A73E3649821}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Define either nmolar or ngmL
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{774B5792-4D0A-424F-8698-961764A4C201}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Define either ngmL or nmolar
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -890,7 +927,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="71">
   <si>
     <t>analysis_id</t>
   </si>
@@ -1098,10 +1135,13 @@
     <t xml:space="preserve">  Version 0.19</t>
   </si>
   <si>
-    <t>chemical_formula</t>
-  </si>
-  <si>
     <t>molecular_weight</t>
+  </si>
+  <si>
+    <t>istd_conc_ngml</t>
+  </si>
+  <si>
+    <t>chem_formula</t>
   </si>
 </sst>
 </file>
@@ -2641,7 +2681,7 @@
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2671,10 +2711,10 @@
         <v>23</v>
       </c>
       <c r="E1" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="21" t="s">
         <v>68</v>
-      </c>
-      <c r="F1" s="21" t="s">
-        <v>69</v>
       </c>
       <c r="G1" s="21" t="s">
         <v>9</v>
@@ -2709,22 +2749,25 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2781,7 +2824,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fix quantifier col in metadata xlsx template
</commit_message>
<xml_diff>
--- a/inst/extdata/midar_metadata_templates.xlsx
+++ b/inst/extdata/midar_metadata_templates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10407"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lsibjb/Documents/Code/midar/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1679488-CED5-304E-8E14-5C24EE10EC78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20A1C2A-B631-9C43-840C-8EB1C11AD8B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13060" yWindow="3140" windowWidth="22940" windowHeight="19140" activeTab="2" xr2:uid="{7A04E2C8-868F-5640-98CB-88D372530A12}"/>
   </bookViews>
@@ -962,9 +962,6 @@
     <t>response_factor</t>
   </si>
   <si>
-    <t>quantifier</t>
-  </si>
-  <si>
     <t>valid_integration</t>
   </si>
   <si>
@@ -1142,6 +1139,9 @@
   </si>
   <si>
     <t>chem_formula</t>
+  </si>
+  <si>
+    <t>is_quantifier</t>
   </si>
 </sst>
 </file>
@@ -2357,73 +2357,73 @@
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="44" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" s="26"/>
       <c r="C7" s="26"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="44" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B13" s="17"/>
       <c r="C13" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -2431,7 +2431,7 @@
     </row>
     <row r="15" spans="1:3" s="8" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:3" s="8" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.2">
@@ -2439,73 +2439,73 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="C20" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="C21" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="C22" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="10" customHeight="1" x14ac:dyDescent="0.2">
@@ -2519,7 +2519,7 @@
     </row>
     <row r="27" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
@@ -2527,7 +2527,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
@@ -2535,7 +2535,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
@@ -2543,7 +2543,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
@@ -2557,7 +2557,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
@@ -2565,7 +2565,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
@@ -2573,7 +2573,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
@@ -2587,7 +2587,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
@@ -2595,7 +2595,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
@@ -2652,7 +2652,7 @@
         <v>5</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E1" s="21" t="s">
         <v>2</v>
@@ -2664,7 +2664,7 @@
         <v>4</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -2681,7 +2681,7 @@
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2708,13 +2708,13 @@
         <v>8</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G1" s="21" t="s">
         <v>9</v>
@@ -2723,19 +2723,19 @@
         <v>10</v>
       </c>
       <c r="I1" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="K1" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="L1" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="M1" s="21" t="s">
         <v>14</v>
-      </c>
-      <c r="M1" s="21" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -2762,13 +2762,13 @@
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -2801,13 +2801,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2837,16 +2837,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add Regression Param columns
</commit_message>
<xml_diff>
--- a/inst/extdata/midar_metadata_templates.xlsx
+++ b/inst/extdata/midar_metadata_templates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10407"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lsibjb/Documents/Code/midar/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1679488-CED5-304E-8E14-5C24EE10EC78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D1A804-2E7F-9A42-AF65-F45D8BC369B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13060" yWindow="3140" windowWidth="22940" windowHeight="19140" activeTab="2" xr2:uid="{7A04E2C8-868F-5640-98CB-88D372530A12}"/>
+    <workbookView xWindow="13060" yWindow="3140" windowWidth="22940" windowHeight="19140" xr2:uid="{7A04E2C8-868F-5640-98CB-88D372530A12}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="6" r:id="rId1"/>
@@ -763,6 +763,34 @@
         </r>
       </text>
     </comment>
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{0B3BC74F-042E-D940-8ED2-CE367BFE1CE6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Either 'linear' or 'quadratic'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{1BE932C9-295D-1049-B7C7-2AA12E6D503E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Either '1/x', '1/x2' or 'none'</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -927,7 +955,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="73">
   <si>
     <t>analysis_id</t>
   </si>
@@ -1142,6 +1170,12 @@
   </si>
   <si>
     <t>chem_formula</t>
+  </si>
+  <si>
+    <t>Curve_Fit_Model</t>
+  </si>
+  <si>
+    <t>Curve_Fit_Weighting</t>
   </si>
 </sst>
 </file>
@@ -2343,7 +2377,7 @@
   </sheetPr>
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
@@ -2678,10 +2712,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2694,10 +2728,11 @@
     <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="20.6640625" customWidth="1"/>
+    <col min="15" max="15" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
         <v>6</v>
       </c>
@@ -2735,6 +2770,12 @@
         <v>14</v>
       </c>
       <c r="M1" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="O1" s="21" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
support exclude QC data points
</commit_message>
<xml_diff>
--- a/inst/extdata/midar_metadata_templates.xlsx
+++ b/inst/extdata/midar_metadata_templates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lsibjb/Documents/Code/midar/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ABB4BA7-BF00-DA41-B5F2-360533B8D286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313392B6-7508-D047-BE3B-4C40613EA2F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13060" yWindow="3140" windowWidth="22940" windowHeight="19140" xr2:uid="{7A04E2C8-868F-5640-98CB-88D372530A12}"/>
   </bookViews>
@@ -922,12 +922,38 @@
         </r>
       </text>
     </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{14BC61A4-4873-8F42-B3D1-93092B22F15D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Unit of the concentration given in the column "concentration"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{608C44CB-EA0C-1944-8482-E7A9EEA64394}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Empty  or TRUE means this data point will be used in an calculation using this table, such as calibration regression and calculation of bias.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="75">
   <si>
     <t>analysis_id</t>
   </si>
@@ -996,9 +1022,6 @@
   </si>
   <si>
     <t>analyte_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Metadata templates for Midar </t>
   </si>
   <si>
     <t>valid_analysis</t>
@@ -1129,9 +1152,6 @@
     <t xml:space="preserve">https://slinghub.github.io/midar/ </t>
   </si>
   <si>
-    <t xml:space="preserve">  Version 0.19</t>
-  </si>
-  <si>
     <t>molecular_weight</t>
   </si>
   <si>
@@ -1142,6 +1162,24 @@
   </si>
   <si>
     <t>is_quantifier</t>
+  </si>
+  <si>
+    <t>include_in_analysis</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>0.2.3</t>
+  </si>
+  <si>
+    <t>Last Update</t>
+  </si>
+  <si>
+    <t>27.06.2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metadata templates for MiDAR </t>
   </si>
 </sst>
 </file>
@@ -2010,8 +2048,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{96874412-AD02-9E4A-97E9-66911C2CB37D}" name="Table1" displayName="Table1" ref="A17:C22" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A17:C22" xr:uid="{96874412-AD02-9E4A-97E9-66911C2CB37D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{96874412-AD02-9E4A-97E9-66911C2CB37D}" name="Table1" displayName="Table1" ref="A19:C24" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A19:C24" xr:uid="{96874412-AD02-9E4A-97E9-66911C2CB37D}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{A4EB99F3-C8C8-2743-9E21-4B41CC03EBBD}" name="Table" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{D255B7CE-69B8-D645-9664-F52D9E285D4B}" name="function of midar used to import" dataDxfId="1"/>
@@ -2341,10 +2379,10 @@
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2357,262 +2395,277 @@
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="18" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="3" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
+    <row r="9" spans="1:3" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="14" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="14" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="24" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="17"/>
+      <c r="C15" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
-    </row>
-    <row r="15" spans="1:3" s="8" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" s="8" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="7"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="25" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="9" t="s">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="6"/>
+    </row>
+    <row r="17" spans="1:4" s="8" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="8" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="7"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>33</v>
+      <c r="C19" s="25" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="C24" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A24" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="10" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="10"/>
-    </row>
-    <row r="26" spans="1:4" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="11"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-    </row>
-    <row r="27" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
+    </row>
+    <row r="26" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A26" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="10"/>
+    </row>
+    <row r="28" spans="1:4" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
       <c r="D28" s="11"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
+    <row r="29" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
       <c r="D29" s="11"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
       <c r="D30" s="11"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="12"/>
+      <c r="A31" s="12" t="s">
+        <v>49</v>
+      </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
       <c r="D31" s="11"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="13" t="s">
-        <v>56</v>
+      <c r="A32" s="12" t="s">
+        <v>51</v>
       </c>
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
       <c r="D32" s="11"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="12" t="s">
-        <v>53</v>
-      </c>
+      <c r="A33" s="12"/>
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
       <c r="D33" s="11"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="12" t="s">
-        <v>54</v>
+      <c r="A34" s="13" t="s">
+        <v>55</v>
       </c>
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
       <c r="D34" s="11"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="12"/>
+      <c r="A35" s="12" t="s">
+        <v>52</v>
+      </c>
       <c r="B35" s="12"/>
       <c r="C35" s="12"/>
       <c r="D35" s="11"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="13" t="s">
-        <v>57</v>
+      <c r="A36" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
       <c r="D36" s="11"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="12" t="s">
-        <v>55</v>
-      </c>
+      <c r="A37" s="12"/>
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
       <c r="D37" s="11"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="12"/>
+      <c r="A38" s="13" t="s">
+        <v>56</v>
+      </c>
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
       <c r="D38" s="11"/>
     </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="11"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="12"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="11"/>
+    </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
-    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A9:C9"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C13" r:id="rId1" xr:uid="{E3824E0A-C653-F742-B26D-1B40EC116563}"/>
+    <hyperlink ref="C15" r:id="rId1" xr:uid="{E3824E0A-C653-F742-B26D-1B40EC116563}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2664,7 +2717,7 @@
         <v>4</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2711,10 +2764,10 @@
         <v>22</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G1" s="21" t="s">
         <v>9</v>
@@ -2723,7 +2776,7 @@
         <v>10</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J1" s="21" t="s">
         <v>11</v>
@@ -2765,7 +2818,7 @@
         <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D1" t="s">
         <v>14</v>
@@ -2821,10 +2874,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2835,7 +2888,7 @@
     <col min="4" max="4" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -2847,6 +2900,9 @@
       </c>
       <c r="D1" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>